<commit_message>
adicionado calculo do gap em segundos
</commit_message>
<xml_diff>
--- a/Alisson/Calculos do transito.xlsx
+++ b/Alisson/Calculos do transito.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28308"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BCE9D0F0-C092-436C-8B63-CA179A26A6D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{92738481-DC3D-479A-9F47-E94FE2100AF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -85,7 +85,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -122,8 +122,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="20">
+  <borders count="23">
     <border>
       <left/>
       <right/>
@@ -145,19 +151,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color rgb="FF000000"/>
       </left>
@@ -225,17 +218,6 @@
         <color rgb="FF000000"/>
       </top>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -287,6 +269,19 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right style="medium">
+        <color theme="1"/>
+      </right>
+      <top style="medium">
+        <color theme="1"/>
+      </top>
+      <bottom style="medium">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="medium">
         <color theme="1"/>
       </left>
@@ -298,10 +293,32 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right style="medium">
+        <color theme="1"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="medium">
         <color theme="1"/>
       </left>
       <right/>
+      <top style="medium">
+        <color theme="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color theme="1"/>
+      </right>
       <top style="medium">
         <color theme="1"/>
       </top>
@@ -348,121 +365,150 @@
       <bottom style="medium">
         <color theme="1"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color theme="1"/>
+      </right>
+      <top/>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -797,195 +843,341 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="C2:P20"/>
+  <dimension ref="A1:Q20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="4" max="4" width="22.7109375" customWidth="1"/>
-    <col min="9" max="9" width="15.85546875" customWidth="1"/>
+    <col min="3" max="3" width="22.7109375" customWidth="1"/>
+    <col min="8" max="8" width="15.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:16">
-      <c r="C2" s="29" t="s">
+    <row r="1" spans="1:17">
+      <c r="A1" s="39"/>
+      <c r="B1" s="40"/>
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
+      <c r="E1" s="40"/>
+      <c r="F1" s="40"/>
+      <c r="G1" s="40"/>
+      <c r="H1" s="40"/>
+      <c r="I1" s="40"/>
+      <c r="J1" s="40"/>
+      <c r="K1" s="40"/>
+      <c r="L1" s="40"/>
+      <c r="M1" s="40"/>
+      <c r="N1" s="40"/>
+      <c r="O1" s="40"/>
+      <c r="P1" s="40"/>
+      <c r="Q1" s="41"/>
+    </row>
+    <row r="2" spans="1:17">
+      <c r="A2" s="42"/>
+      <c r="B2" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="35"/>
-      <c r="E2" s="36">
+      <c r="C2" s="28"/>
+      <c r="D2" s="29">
         <v>120</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="I2" s="7"/>
-      <c r="J2" s="5">
+      <c r="H2" s="4"/>
+      <c r="I2" s="2">
         <v>2</v>
       </c>
-      <c r="M2" s="13"/>
-      <c r="N2" s="1" t="s">
+      <c r="J2" s="38"/>
+      <c r="K2" s="38"/>
+      <c r="L2" s="48"/>
+      <c r="M2" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="O2" s="4"/>
-      <c r="P2" s="2"/>
-    </row>
-    <row r="3" spans="3:16">
-      <c r="C3" s="30" t="s">
+      <c r="N2" s="47"/>
+      <c r="O2" s="25"/>
+      <c r="P2" s="38"/>
+      <c r="Q2" s="43"/>
+    </row>
+    <row r="3" spans="1:17">
+      <c r="A3" s="42"/>
+      <c r="B3" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="37"/>
-      <c r="E3" s="28">
+      <c r="C3" s="30"/>
+      <c r="D3" s="19">
         <v>6</v>
       </c>
-      <c r="H3" s="8" t="s">
+      <c r="E3" s="38"/>
+      <c r="F3" s="38"/>
+      <c r="G3" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="I3" s="9"/>
-      <c r="J3" s="3">
+      <c r="H3" s="6"/>
+      <c r="I3" s="1">
         <v>1</v>
       </c>
-      <c r="M3" s="12"/>
-      <c r="N3" s="4" t="s">
+      <c r="J3" s="38"/>
+      <c r="K3" s="38"/>
+      <c r="L3" s="9"/>
+      <c r="M3" s="49" t="s">
         <v>5</v>
       </c>
-      <c r="O3" s="4"/>
-      <c r="P3" s="2"/>
-    </row>
-    <row r="4" spans="3:16">
-      <c r="C4" s="21"/>
-      <c r="D4" s="21"/>
-      <c r="E4" s="22"/>
-      <c r="H4" s="21"/>
-      <c r="I4" s="21"/>
-      <c r="J4" s="20"/>
-      <c r="M4" s="24"/>
-      <c r="N4" s="14" t="s">
+      <c r="N3" s="49"/>
+      <c r="O3" s="50"/>
+      <c r="P3" s="38"/>
+      <c r="Q3" s="43"/>
+    </row>
+    <row r="4" spans="1:17">
+      <c r="A4" s="42"/>
+      <c r="B4" s="37"/>
+      <c r="C4" s="37"/>
+      <c r="D4" s="38"/>
+      <c r="E4" s="38"/>
+      <c r="F4" s="38"/>
+      <c r="G4" s="37"/>
+      <c r="H4" s="37"/>
+      <c r="I4" s="38"/>
+      <c r="J4" s="38"/>
+      <c r="K4" s="38"/>
+      <c r="L4" s="52"/>
+      <c r="M4" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="O4" s="15"/>
-      <c r="P4" s="16"/>
-    </row>
-    <row r="5" spans="3:16">
-      <c r="C5" s="32" t="s">
+      <c r="N4" s="11"/>
+      <c r="O4" s="12"/>
+      <c r="P4" s="38"/>
+      <c r="Q4" s="43"/>
+    </row>
+    <row r="5" spans="1:17">
+      <c r="A5" s="42"/>
+      <c r="B5" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="38"/>
-      <c r="E5" s="36">
-        <f>E2/3.6</f>
+      <c r="C5" s="31"/>
+      <c r="D5" s="29">
+        <f>D2/3.6</f>
         <v>33.333333333333336</v>
       </c>
-      <c r="H5" s="26" t="s">
+      <c r="E5" s="38"/>
+      <c r="F5" s="38"/>
+      <c r="G5" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="I5" s="27"/>
-      <c r="J5" s="5">
-        <f>(E3/((E7-E6)/1000))*3.6</f>
+      <c r="H5" s="18"/>
+      <c r="I5" s="2">
+        <f>(D3/((D7-D6)/1000))*3.6</f>
         <v>120.00000000000001</v>
       </c>
-      <c r="M5" s="25"/>
-      <c r="N5" s="17"/>
-      <c r="O5" s="18"/>
-      <c r="P5" s="19"/>
-    </row>
-    <row r="6" spans="3:16">
-      <c r="C6" s="32" t="s">
+      <c r="J5" s="38"/>
+      <c r="K5" s="38"/>
+      <c r="L5" s="51"/>
+      <c r="M5" s="13"/>
+      <c r="N5" s="13"/>
+      <c r="O5" s="14"/>
+      <c r="P5" s="38"/>
+      <c r="Q5" s="43"/>
+    </row>
+    <row r="6" spans="1:17">
+      <c r="A6" s="42"/>
+      <c r="B6" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="38"/>
-      <c r="E6" s="36">
-        <f>J2/E5*1000</f>
+      <c r="C6" s="31"/>
+      <c r="D6" s="29">
+        <f>I2/D5*1000</f>
         <v>60</v>
       </c>
-      <c r="H6" s="10" t="s">
+      <c r="E6" s="38"/>
+      <c r="F6" s="38"/>
+      <c r="G6" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="I6" s="11"/>
-      <c r="J6" s="3">
-        <f>E5*((E7-E6)/1000)</f>
+      <c r="H6" s="8"/>
+      <c r="I6" s="1">
+        <f>D5*((D7-D6)/1000)</f>
         <v>6</v>
       </c>
-    </row>
-    <row r="7" spans="3:16">
-      <c r="C7" s="32" t="s">
+      <c r="J6" s="38"/>
+      <c r="K6" s="38"/>
+      <c r="L6" s="38"/>
+      <c r="M6" s="38"/>
+      <c r="N6" s="38"/>
+      <c r="O6" s="38"/>
+      <c r="P6" s="38"/>
+      <c r="Q6" s="43"/>
+    </row>
+    <row r="7" spans="1:17">
+      <c r="A7" s="42"/>
+      <c r="B7" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="38"/>
-      <c r="E7" s="36">
-        <f>((E3*1000000)/(E5*1000))+E6</f>
+      <c r="C7" s="31"/>
+      <c r="D7" s="29">
+        <f>((D3*1000000)/(D5*1000))+D6</f>
         <v>240</v>
       </c>
-    </row>
-    <row r="8" spans="3:16">
-      <c r="C8" s="31" t="s">
+      <c r="E7" s="38"/>
+      <c r="F7" s="38"/>
+      <c r="G7" s="38"/>
+      <c r="H7" s="38"/>
+      <c r="I7" s="38"/>
+      <c r="J7" s="38"/>
+      <c r="K7" s="38"/>
+      <c r="L7" s="38"/>
+      <c r="M7" s="38"/>
+      <c r="N7" s="38"/>
+      <c r="O7" s="38"/>
+      <c r="P7" s="38"/>
+      <c r="Q7" s="43"/>
+    </row>
+    <row r="8" spans="1:17">
+      <c r="A8" s="42"/>
+      <c r="B8" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="39"/>
-      <c r="E8" s="28">
-        <f>(J2+J3)*E5</f>
+      <c r="C8" s="32"/>
+      <c r="D8" s="19">
+        <f>(I2+I3)*D5</f>
         <v>100</v>
       </c>
-    </row>
-    <row r="10" spans="3:16">
-      <c r="C10" s="33" t="s">
+      <c r="E8" s="38"/>
+      <c r="F8" s="38"/>
+      <c r="G8" s="38"/>
+      <c r="H8" s="38"/>
+      <c r="I8" s="38"/>
+      <c r="J8" s="38"/>
+      <c r="K8" s="38"/>
+      <c r="L8" s="38"/>
+      <c r="M8" s="38"/>
+      <c r="N8" s="38"/>
+      <c r="O8" s="38"/>
+      <c r="P8" s="38"/>
+      <c r="Q8" s="43"/>
+    </row>
+    <row r="9" spans="1:17">
+      <c r="A9" s="42"/>
+      <c r="B9" s="38"/>
+      <c r="C9" s="38"/>
+      <c r="D9" s="38"/>
+      <c r="E9" s="38"/>
+      <c r="F9" s="38"/>
+      <c r="G9" s="38"/>
+      <c r="H9" s="38"/>
+      <c r="I9" s="38"/>
+      <c r="J9" s="38"/>
+      <c r="K9" s="38"/>
+      <c r="L9" s="38"/>
+      <c r="M9" s="38"/>
+      <c r="N9" s="38"/>
+      <c r="O9" s="38"/>
+      <c r="P9" s="38"/>
+      <c r="Q9" s="43"/>
+    </row>
+    <row r="10" spans="1:17">
+      <c r="A10" s="42"/>
+      <c r="B10" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="D10" s="34"/>
-      <c r="E10" s="36">
+      <c r="C10" s="27"/>
+      <c r="D10" s="29">
         <v>60</v>
       </c>
-      <c r="H10" s="40" t="s">
+      <c r="E10" s="38"/>
+      <c r="F10" s="38"/>
+      <c r="G10" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="I10" s="41"/>
-      <c r="J10" s="36">
-        <f>(J2/(E10/1000))*3.6</f>
+      <c r="H10" s="34"/>
+      <c r="I10" s="29">
+        <f>(I2/(D10/1000))*3.6</f>
         <v>120.00000000000001</v>
       </c>
-    </row>
-    <row r="11" spans="3:16">
-      <c r="C11" s="29" t="s">
+      <c r="J10" s="38"/>
+      <c r="K10" s="38"/>
+      <c r="L10" s="38"/>
+      <c r="M10" s="38"/>
+      <c r="N10" s="38"/>
+      <c r="O10" s="38"/>
+      <c r="P10" s="38"/>
+      <c r="Q10" s="43"/>
+    </row>
+    <row r="11" spans="1:17">
+      <c r="A11" s="42"/>
+      <c r="B11" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="D11" s="35"/>
-      <c r="E11" s="28">
+      <c r="C11" s="28"/>
+      <c r="D11" s="19">
         <v>240</v>
       </c>
-      <c r="H11" s="42" t="s">
+      <c r="E11" s="38"/>
+      <c r="F11" s="38"/>
+      <c r="G11" s="35" t="s">
         <v>10</v>
       </c>
-      <c r="I11" s="43"/>
-      <c r="J11" s="28">
-        <f>((E11-E10)/1000)*(J10/3.6)</f>
+      <c r="H11" s="36"/>
+      <c r="I11" s="19">
+        <f>((D11-D10)/1000)*(I10/3.6)</f>
         <v>6</v>
       </c>
-    </row>
-    <row r="17" spans="4:9">
-      <c r="D17" s="20"/>
-      <c r="I17" s="20"/>
-    </row>
-    <row r="20" spans="4:9">
-      <c r="F20" s="23"/>
+      <c r="J11" s="38"/>
+      <c r="K11" s="38"/>
+      <c r="L11" s="38"/>
+      <c r="M11" s="38"/>
+      <c r="N11" s="38"/>
+      <c r="O11" s="38"/>
+      <c r="P11" s="38"/>
+      <c r="Q11" s="43"/>
+    </row>
+    <row r="12" spans="1:17">
+      <c r="A12" s="44"/>
+      <c r="B12" s="45"/>
+      <c r="C12" s="45"/>
+      <c r="D12" s="45"/>
+      <c r="E12" s="45"/>
+      <c r="F12" s="45"/>
+      <c r="G12" s="45"/>
+      <c r="H12" s="45"/>
+      <c r="I12" s="45"/>
+      <c r="J12" s="45"/>
+      <c r="K12" s="45"/>
+      <c r="L12" s="45"/>
+      <c r="M12" s="45"/>
+      <c r="N12" s="45"/>
+      <c r="O12" s="45"/>
+      <c r="P12" s="45"/>
+      <c r="Q12" s="46"/>
+    </row>
+    <row r="17" spans="3:8">
+      <c r="C17" s="15"/>
+      <c r="H17" s="15"/>
+    </row>
+    <row r="20" spans="3:8">
+      <c r="E20" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="H10:I10"/>
-    <mergeCell ref="H11:I11"/>
-    <mergeCell ref="N3:P3"/>
-    <mergeCell ref="N2:P2"/>
-    <mergeCell ref="N4:P5"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="M3:O3"/>
+    <mergeCell ref="M2:O2"/>
+    <mergeCell ref="M4:O5"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="B6:C6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>